<commit_message>
wersja alfa 1.5.2a; małe poprawki
</commit_message>
<xml_diff>
--- a/Kopia pliku WZÓR - GRAFIK (INDYWIDUALNY ROZKŁAD CZASU PRACY PRACOWNIKÓW).xlsx
+++ b/Kopia pliku WZÓR - GRAFIK (INDYWIDUALNY ROZKŁAD CZASU PRACY PRACOWNIKÓW).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\ITEGER\staż\obecności\All_Reader\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\ITEGER\staż\obecności\All_Reader\Pliki pokaz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BC5023-23AA-496C-8A82-265BF1F0E042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C335E9-32EA-4C4A-8A55-D55233293F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10185" yWindow="270" windowWidth="18615" windowHeight="14895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1305" windowWidth="18615" windowHeight="14895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="listopad 2024-2" sheetId="20" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="12">
   <si>
     <t>Godziny pracy od</t>
   </si>
@@ -51,12 +51,6 @@
     <t>Data</t>
   </si>
   <si>
-    <t>Nazwisko Imię</t>
-  </si>
-  <si>
-    <t>akronim</t>
-  </si>
-  <si>
     <t>DW5</t>
   </si>
   <si>
@@ -66,7 +60,13 @@
     <t>Ś</t>
   </si>
   <si>
-    <t>Norbert Tasarz</t>
+    <t>Hetman Paweł</t>
+  </si>
+  <si>
+    <t>Miros Łukasz</t>
+  </si>
+  <si>
+    <t>Piekart Paweł</t>
   </si>
 </sst>
 </file>
@@ -694,6 +694,43 @@
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
@@ -708,43 +745,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
   </cellXfs>
@@ -1200,7 +1200,7 @@
   <dimension ref="A1:M1307"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1210,119 +1210,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="53" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="54"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="53" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="54"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="53" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="54"/>
-      <c r="M1" s="55"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="50"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="50"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="51"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" s="43"/>
       <c r="C2" s="44">
-        <v>211521</v>
+        <v>59224</v>
       </c>
       <c r="D2" s="45"/>
       <c r="E2" s="43"/>
-      <c r="F2" s="44" t="s">
-        <v>7</v>
+      <c r="F2" s="44">
+        <v>57450</v>
       </c>
       <c r="G2" s="45"/>
       <c r="H2" s="43"/>
-      <c r="I2" s="44" t="s">
-        <v>7</v>
+      <c r="I2" s="44">
+        <v>52044</v>
       </c>
       <c r="J2" s="45"/>
       <c r="K2" s="43"/>
-      <c r="L2" s="44" t="s">
-        <v>7</v>
-      </c>
+      <c r="L2" s="44"/>
       <c r="M2" s="45"/>
     </row>
     <row r="3" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="D3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="58" t="s">
+      <c r="F3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="60" t="s">
+      <c r="G3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="56" t="s">
+      <c r="H3" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="58" t="s">
+      <c r="I3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="60" t="s">
+      <c r="J3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="56" t="s">
+      <c r="K3" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="L3" s="58" t="s">
+      <c r="L3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="60" t="s">
+      <c r="M3" s="56" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="51"/>
-      <c r="B4" s="57"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="59"/>
-      <c r="M4" s="61"/>
+      <c r="A4" s="61"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="55"/>
+      <c r="M4" s="57"/>
     </row>
     <row r="5" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="52"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="57"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="62"/>
-      <c r="K5" s="57"/>
-      <c r="L5" s="59"/>
-      <c r="M5" s="62"/>
+      <c r="A5" s="62"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="55"/>
+      <c r="M5" s="58"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="25">
@@ -1373,16 +1369,24 @@
         <v>0.625</v>
       </c>
       <c r="C7" s="32">
-        <v>0.83333333333333337</v>
+        <v>0.84375</v>
       </c>
       <c r="D7" s="33">
         <v>8</v>
       </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="14"/>
+      <c r="E7" s="13">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="F7" s="14">
+        <v>0.4375</v>
+      </c>
       <c r="G7" s="15"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="14"/>
+      <c r="H7" s="13">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="I7" s="14">
+        <v>0.95833333333333337</v>
+      </c>
       <c r="J7" s="15"/>
       <c r="K7" s="13"/>
       <c r="L7" s="14"/>
@@ -1405,7 +1409,7 @@
       <c r="L8" s="2"/>
       <c r="M8" s="16"/>
     </row>
-    <row r="9" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27">
         <v>45599</v>
       </c>
@@ -1432,12 +1436,8 @@
       <c r="E10" s="6"/>
       <c r="F10" s="2"/>
       <c r="G10" s="16"/>
-      <c r="H10" s="6">
-        <v>0.625</v>
-      </c>
-      <c r="I10" s="32">
-        <v>0.83333333333333337</v>
-      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="2"/>
       <c r="J10" s="16"/>
       <c r="K10" s="6"/>
       <c r="L10" s="2"/>
@@ -1468,10 +1468,10 @@
       <c r="C12" s="35"/>
       <c r="D12" s="36"/>
       <c r="E12" s="6">
-        <v>2.0833333333333333E-3</v>
-      </c>
-      <c r="F12" s="6">
-        <v>0.625</v>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.95833333333333337</v>
       </c>
       <c r="G12" s="16"/>
       <c r="H12" s="6"/>
@@ -1511,12 +1511,8 @@
       <c r="H14" s="13"/>
       <c r="I14" s="14"/>
       <c r="J14" s="15"/>
-      <c r="K14" s="13">
-        <v>0.46736111111111112</v>
-      </c>
-      <c r="L14" s="32">
-        <v>0.83333333333333337</v>
-      </c>
+      <c r="K14" s="13"/>
+      <c r="L14" s="32"/>
       <c r="M14" s="15"/>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1966,7 +1962,7 @@
     <row r="41" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="46"/>
       <c r="B41" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
@@ -1975,7 +1971,7 @@
     <row r="42" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="48"/>
       <c r="B42" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
@@ -1984,7 +1980,7 @@
     <row r="43" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="47"/>
       <c r="B43" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
@@ -2005,17 +2001,17 @@
       <c r="E45" s="1"/>
     </row>
     <row r="46" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="49"/>
-      <c r="B46" s="49"/>
-      <c r="C46" s="49"/>
-      <c r="D46" s="49"/>
+      <c r="A46" s="59"/>
+      <c r="B46" s="59"/>
+      <c r="C46" s="59"/>
+      <c r="D46" s="59"/>
       <c r="E46" s="5"/>
     </row>
     <row r="47" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="49"/>
-      <c r="B47" s="49"/>
-      <c r="C47" s="49"/>
-      <c r="D47" s="49"/>
+      <c r="A47" s="59"/>
+      <c r="B47" s="59"/>
+      <c r="C47" s="59"/>
+      <c r="D47" s="59"/>
       <c r="E47" s="5"/>
     </row>
     <row r="48" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3280,14 +3276,6 @@
     <row r="1307" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="H3:H5"/>
-    <mergeCell ref="I3:I5"/>
-    <mergeCell ref="J3:J5"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="K3:K5"/>
-    <mergeCell ref="L3:L5"/>
-    <mergeCell ref="M3:M5"/>
     <mergeCell ref="A46:D47"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B1:D1"/>
@@ -3298,6 +3286,14 @@
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="D3:D5"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="H3:H5"/>
+    <mergeCell ref="I3:I5"/>
+    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="K3:K5"/>
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="M3:M5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>